<commit_message>
FIX: Dates are only valid up to the last day of 9999
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/DAY.xlsx
+++ b/xlsx/tests/docs/DAY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\Function descriptions\Date and Time\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\DAY-MONTH-YEAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB85CF6F-90D4-4971-8B3B-6398E0E87083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D9427F-AF3E-428E-882A-C350F9DA6A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7E191B1-44A3-4478-A86F-CB5CE7E3580C}"/>
+    <workbookView xWindow="4215" yWindow="2100" windowWidth="22200" windowHeight="11595" xr2:uid="{C7E191B1-44A3-4478-A86F-CB5CE7E3580C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,33 +36,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Day()</t>
-  </si>
-  <si>
     <t>Cell reference</t>
   </si>
   <si>
     <t>Using DATE function</t>
   </si>
   <si>
-    <t>Date literal</t>
-  </si>
-  <si>
     <t>Integer serial number</t>
   </si>
   <si>
     <t>Serial number with fractional part</t>
+  </si>
+  <si>
+    <t>Formula Text</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>DAY()</t>
+  </si>
+  <si>
+    <t>Largest serial number that can be formatted as a date</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Example of error propagation.</t>
+  </si>
+  <si>
+    <t>Input causes a #DIV/0! error.</t>
+  </si>
+  <si>
+    <t>Unable to convert date argument to a number.</t>
+  </si>
+  <si>
+    <t>Negative serial number.</t>
+  </si>
+  <si>
+    <t>Date literal (short date)</t>
+  </si>
+  <si>
+    <t>Date literal (ISO 8601)</t>
+  </si>
+  <si>
+    <t>Lowest accepted serial number</t>
+  </si>
+  <si>
+    <t>Serial number too large.</t>
+  </si>
+  <si>
+    <t>Should error - 1900 is not a leap year.</t>
+  </si>
+  <si>
+    <t>Largest serial number accepted by DAY (31/12/262142)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,12 +122,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,12 +148,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,79 +503,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6100931E-B86C-4134-94C5-0A5BD3A5B1E4}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>45651</v>
+      </c>
+      <c r="B2" s="2">
+        <f>DAY(A2)</f>
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B2)</f>
+        <v>=DAY(A2)</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>45619</v>
-      </c>
-      <c r="B2">
-        <f>DAY(A2)</f>
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2">
+        <f>DAY(DATE(2024,12,25))</f>
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f t="shared" ref="C3:C13" ca="1" si="0">_xlfn.FORMULATEXT(B3)</f>
+        <v>=DAY(DATE(2024,12,25))</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <f>DAY(DATE(2024, 11, 23))</f>
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <f>DAY("2024-11-23")</f>
-        <v>23</v>
+      <c r="A4" s="4"/>
+      <c r="B4" s="2">
+        <f>DAY("2024-12-25")</f>
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=DAY("2024-12-25")</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>45619</v>
-      </c>
-      <c r="B5">
-        <f>DAY(A5)</f>
-        <v>23</v>
+      <c r="A5" s="4"/>
+      <c r="B5" s="2">
+        <f>DAY("25/12/2024")</f>
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=DAY("25/12/2024")</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>45619.9</v>
-      </c>
-      <c r="B6">
+        <v>45651</v>
+      </c>
+      <c r="B6" s="2">
         <f>DAY(A6)</f>
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=DAY(A6)</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>45651.9</v>
+      </c>
+      <c r="B7" s="2">
+        <f>DAY(A7)</f>
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=DAY(A7)</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2">
+        <f>DAY(A9)</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B9)</f>
+        <v>=DAY(A9)</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <f>DAY(A10)</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B10)</f>
+        <v>=DAY(A10)</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>61</v>
+      </c>
+      <c r="B11" s="2">
+        <f>DAY(A11)</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B11)</f>
+        <v>=DAY(A11)</v>
+      </c>
+      <c r="D11" s="7">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>2958465</v>
+      </c>
+      <c r="B12" s="2">
+        <f>DAY(A12)</f>
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=DAY(A12)</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>95051805</v>
+      </c>
+      <c r="B13" s="2" t="e">
+        <f>DAY(A13)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=DAY(A13)</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="e">
+        <f>DAY(SQRT(-1))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A17)</f>
+        <v>=DAY(SQRT(-1))</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="e">
+        <f>DAY("str")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B18" s="3" t="str">
+        <f t="shared" ref="B18:B19" ca="1" si="1">_xlfn.FORMULATEXT(A18)</f>
+        <v>=DAY("str")</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="e">
+        <f>DAY(10/0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B19" s="3" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=DAY(10/0)</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="e">
+        <f>DAY(-1)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B20" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A20)</f>
+        <v>=DAY(-1)</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="e">
+        <f>DAY(95051806)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B21" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A21)</f>
+        <v>=DAY(95051806)</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <f>DAY(DATE(1900,2,29))</f>
+        <v>29</v>
+      </c>
+      <c r="B22" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A22)</f>
+        <v>=DAY(DATE(1900,2,29))</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add DAY function description
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/DAY.xlsx
+++ b/xlsx/tests/docs/DAY.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\DAY-MONTH-YEAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\IronCalc-clone\IronCalc-SF\xlsx\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D9427F-AF3E-428E-882A-C350F9DA6A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2B09AD-CE00-4195-9C3A-DE8EA18711C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="2100" windowWidth="22200" windowHeight="11595" xr2:uid="{C7E191B1-44A3-4478-A86F-CB5CE7E3580C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7E191B1-44A3-4478-A86F-CB5CE7E3580C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Comments</t>
   </si>
@@ -62,40 +62,31 @@
     <t>DAY()</t>
   </si>
   <si>
-    <t>Largest serial number that can be formatted as a date</t>
-  </si>
-  <si>
     <t>Formula</t>
   </si>
   <si>
-    <t>Example of error propagation.</t>
-  </si>
-  <si>
-    <t>Input causes a #DIV/0! error.</t>
-  </si>
-  <si>
-    <t>Unable to convert date argument to a number.</t>
-  </si>
-  <si>
-    <t>Negative serial number.</t>
-  </si>
-  <si>
-    <t>Date literal (short date)</t>
-  </si>
-  <si>
-    <t>Date literal (ISO 8601)</t>
-  </si>
-  <si>
-    <t>Lowest accepted serial number</t>
-  </si>
-  <si>
-    <t>Serial number too large.</t>
-  </si>
-  <si>
-    <t>Should error - 1900 is not a leap year.</t>
-  </si>
-  <si>
-    <t>Largest serial number accepted by DAY (31/12/262142)</t>
+    <t>Largest accepted serial number</t>
+  </si>
+  <si>
+    <t>Smallest accepted serial number</t>
+  </si>
+  <si>
+    <t>Excel considers this 29/02/1900 (although 1900 was not a leap year)</t>
+  </si>
+  <si>
+    <t>Example of error propagation</t>
+  </si>
+  <si>
+    <t>Unable to convert date argument to a number</t>
+  </si>
+  <si>
+    <t>Negative serial number</t>
+  </si>
+  <si>
+    <t>Serial number too large</t>
+  </si>
+  <si>
+    <t>Input causes a #DIV/0! error</t>
   </si>
 </sst>
 </file>
@@ -103,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -148,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,15 +150,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,17 +499,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6100931E-B86C-4134-94C5-0A5BD3A5B1E4}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -532,7 +528,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>45651</v>
       </c>
       <c r="B2" s="2">
@@ -548,13 +544,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="2">
         <f>DAY(DATE(2024,12,25))</f>
         <v>25</v>
       </c>
       <c r="C3" s="3" t="str">
-        <f t="shared" ref="C3:C13" ca="1" si="0">_xlfn.FORMULATEXT(B3)</f>
+        <f t="shared" ref="C3:C11" ca="1" si="0">_xlfn.FORMULATEXT(B3)</f>
         <v>=DAY(DATE(2024,12,25))</v>
       </c>
       <c r="D3" t="s">
@@ -562,239 +558,208 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="2">
+        <v>45651</v>
+      </c>
       <c r="B4" s="2">
-        <f>DAY("2024-12-25")</f>
+        <f>DAY(A4)</f>
         <v>25</v>
       </c>
       <c r="C4" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>=DAY("2024-12-25")</v>
+        <v>=DAY(A4)</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="2">
+        <v>45651.9</v>
+      </c>
       <c r="B5" s="2">
-        <f>DAY("25/12/2024")</f>
+        <f>DAY(A5)</f>
         <v>25</v>
       </c>
       <c r="C5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>=DAY("25/12/2024")</v>
+        <v>=DAY(A5)</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>45651</v>
-      </c>
-      <c r="B6" s="2">
-        <f>DAY(A6)</f>
-        <v>25</v>
-      </c>
-      <c r="C6" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>=DAY(A6)</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>45651.9</v>
+      <c r="A7" s="8">
+        <v>0</v>
       </c>
       <c r="B7" s="2">
         <f>DAY(A7)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">_xlfn.FORMULATEXT(B7)</f>
         <v>=DAY(A7)</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <f>DAY(A8)</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B8)</f>
+        <v>=DAY(A8)</v>
+      </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>0</v>
+      <c r="A9" s="8">
+        <v>2</v>
       </c>
       <c r="B9" s="2">
         <f>DAY(A9)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B9)</f>
         <v>=DAY(A9)</v>
       </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>1</v>
+      <c r="A10" s="8">
+        <v>46016</v>
       </c>
       <c r="B10" s="2">
         <f>DAY(A10)</f>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B10)</f>
         <v>=DAY(A10)</v>
       </c>
-      <c r="D10" s="7">
-        <v>1</v>
-      </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>61</v>
+      <c r="A11" s="8">
+        <v>2958465</v>
       </c>
       <c r="B11" s="2">
         <f>DAY(A11)</f>
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B11)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>=DAY(A11)</v>
       </c>
-      <c r="D11" s="7">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>2958465</v>
-      </c>
-      <c r="B12" s="2">
-        <f>DAY(A12)</f>
-        <v>31</v>
-      </c>
-      <c r="C12" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>=DAY(A12)</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>95051805</v>
-      </c>
-      <c r="B13" s="2" t="e">
-        <f>DAY(A13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C13" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>=DAY(A13)</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="e">
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="e">
         <f>DAY(SQRT(-1))</f>
         <v>#NUM!</v>
       </c>
-      <c r="B17" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(A17)</f>
+      <c r="B15" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A15)</f>
         <v>=DAY(SQRT(-1))</v>
       </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="e">
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="e">
         <f>DAY("str")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B18" s="3" t="str">
-        <f t="shared" ref="B18:B19" ca="1" si="1">_xlfn.FORMULATEXT(A18)</f>
+      <c r="B16" s="3" t="str">
+        <f t="shared" ref="B16:B17" ca="1" si="1">_xlfn.FORMULATEXT(A16)</f>
         <v>=DAY("str")</v>
       </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="e">
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="e">
         <f>DAY(10/0)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="B19" s="3" t="str">
+      <c r="B17" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=DAY(10/0)</v>
       </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="e">
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="e">
         <f>DAY(-1)</f>
         <v>#NUM!</v>
       </c>
-      <c r="B20" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(A20)</f>
+      <c r="B18" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A18)</f>
         <v>=DAY(-1)</v>
       </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="e">
-        <f>DAY(95051806)</f>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="e">
+        <f>DAY(2958466)</f>
         <v>#NUM!</v>
       </c>
-      <c r="B21" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(A21)</f>
-        <v>=DAY(95051806)</v>
-      </c>
-      <c r="D21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="B19" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A19)</f>
+        <v>=DAY(2958466)</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <f>DAY(DATE(1900,2,29))</f>
         <v>29</v>
       </c>
-      <c r="B22" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(A22)</f>
+      <c r="B20" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A20)</f>
         <v>=DAY(DATE(1900,2,29))</v>
       </c>
-      <c r="D22" t="s">
-        <v>18</v>
+      <c r="C20" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A15:A19" evalError="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor updates to DAY function page and example spreadsheet
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/DAY.xlsx
+++ b/xlsx/tests/docs/DAY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\IronCalc-clone\IronCalc-SF\xlsx\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2B09AD-CE00-4195-9C3A-DE8EA18711C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07691D3-97E6-4EC6-A3D2-43B3F5484C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7E191B1-44A3-4478-A86F-CB5CE7E3580C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Comments</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Input causes a #DIV/0! error</t>
+  </si>
+  <si>
+    <t>Zero serial number</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +553,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="3" t="str">
-        <f t="shared" ref="C3:C11" ca="1" si="0">_xlfn.FORMULATEXT(B3)</f>
+        <f t="shared" ref="C3:C10" ca="1" si="0">_xlfn.FORMULATEXT(B3)</f>
         <v>=DAY(DATE(2024,12,25))</v>
       </c>
       <c r="D3" t="s">
@@ -595,11 +598,11 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2">
         <f>DAY(A7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B7)</f>
@@ -611,11 +614,11 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2">
         <f>DAY(A8)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B8)</f>
@@ -625,11 +628,11 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <v>2</v>
+        <v>46016</v>
       </c>
       <c r="B9" s="2">
         <f>DAY(A9)</f>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="str">
         <f ca="1">_xlfn.FORMULATEXT(B9)</f>
@@ -639,95 +642,94 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <v>46016</v>
+        <v>2958465</v>
       </c>
       <c r="B10" s="2">
         <f>DAY(A10)</f>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B10)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>=DAY(A10)</v>
       </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>2958465</v>
-      </c>
-      <c r="B11" s="2">
-        <f>DAY(A11)</f>
-        <v>31</v>
-      </c>
-      <c r="C11" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>=DAY(A11)</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
+      <c r="A14" s="5" t="e">
+        <f>DAY(SQRT(-1))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B14" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A14)</f>
+        <v>=DAY(SQRT(-1))</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="e">
-        <f>DAY(SQRT(-1))</f>
-        <v>#NUM!</v>
+        <f>DAY("str")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="B15" s="3" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(A15)</f>
-        <v>=DAY(SQRT(-1))</v>
+        <f t="shared" ref="B15:B16" ca="1" si="1">_xlfn.FORMULATEXT(A15)</f>
+        <v>=DAY("str")</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="e">
-        <f>DAY("str")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="B16" s="3" t="str">
-        <f t="shared" ref="B16:B17" ca="1" si="1">_xlfn.FORMULATEXT(A16)</f>
-        <v>=DAY("str")</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="e">
         <f>DAY(10/0)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="B17" s="3" t="str">
+      <c r="B16" s="3" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=DAY(10/0)</v>
       </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="e">
+        <f>DAY(-5)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A17)</f>
+        <v>=DAY(-5)</v>
+      </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="e">
-        <f>DAY(-1)</f>
-        <v>#NUM!</v>
+      <c r="A18" s="5">
+        <f>DAY(0)</f>
+        <v>0</v>
       </c>
       <c r="B18" s="3" t="str">
         <f ca="1">_xlfn.FORMULATEXT(A18)</f>
-        <v>=DAY(-1)</v>
+        <v>=DAY(0)</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -759,7 +761,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A15:A19" evalError="1"/>
+    <ignoredError sqref="A19 A14:A16" evalError="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>